<commit_message>
Rename name and Add README.md
</commit_message>
<xml_diff>
--- a/ios_testcase.xlsx
+++ b/ios_testcase.xlsx
@@ -28,27 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
-  <si>
-    <t>click</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>我的－首页</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>我的－密码文本框</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="84">
   <si>
     <t/>
   </si>
   <si>
     <t>StartPreview</t>
-  </si>
-  <si>
-    <t>ByAccessibilityId</t>
   </si>
   <si>
     <t>ByAccessibilityId对应元素的name</t>
@@ -252,10 +237,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>click</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>customSleep</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -272,7 +253,236 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ByAccessibilityId</t>
+    <t>findElementByClassName</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Other</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>iosDoubleClick</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>1,1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>findElementByClassName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳转到设置界面</t>
+    <rPh sb="0" eb="1">
+      <t>tiao zhuan</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>dao</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>she zhi</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>jie mian</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PickerWheel</t>
+  </si>
+  <si>
+    <t>pickerWheelChangeTopDefinition</t>
+  </si>
+  <si>
+    <t>滑动到最顶部</t>
+    <rPh sb="0" eb="1">
+      <t>hua dong</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>dao</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>zui ding bu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>findElementsByClassName-0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TextField</t>
+  </si>
+  <si>
+    <t>TextField</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>clear</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sendKeys</t>
+  </si>
+  <si>
+    <t>sendKeys</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>findElementsByClassName-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>findElementsByClassName-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>Apply</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartPreview</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartPush</t>
+  </si>
+  <si>
+    <t>StopPreview</t>
+  </si>
+  <si>
+    <t>StopPush</t>
+  </si>
+  <si>
+    <t>pickerWheechangeDefinition</t>
+  </si>
+  <si>
+    <t>pickerWheechangeDefinition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>customSleep</t>
+  </si>
+  <si>
+    <t>findElementByAccessibilityId</t>
+  </si>
+  <si>
+    <t>defaultSleep</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>findElementsByClassName-4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rtmp://10.2.250.92/live_haibian/024</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>这里点击了Add按钮后, 会自动隐藏键盘, 否则需要手动隐藏键盘</t>
+    <rPh sb="0" eb="1">
+      <t>zhe li</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>dian ji</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>le</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>an niu</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>hui</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>zi dong</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>yin cang</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>jian pan</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>fou ze</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>xu yao</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>shou dong</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>yin cang</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>jian pan</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>iosDoubleClick</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Window</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>findElementsByClassName-6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StaticText</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>findElementsByClassName-8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>assertEquals</t>
+  </si>
+  <si>
+    <t>关闭验证</t>
+    <rPh sb="0" eb="1">
+      <t>guan bi</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yan zheng</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开验证</t>
+    <rPh sb="0" eb="1">
+      <t>d k</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yan zheng</t>
+    </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -280,7 +490,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,6 +663,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF6A8759"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="16.5"/>
+      <color rgb="FF000000"/>
+      <name val="Abadi MT Condensed Extra Bold"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -608,7 +828,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -759,8 +979,254 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -776,8 +1242,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="132">
     <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -802,6 +1277,47 @@
     <cellStyle name="超链接" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="好" xfId="7" builtinId="26" customBuiltin="1"/>
     <cellStyle name="汇总" xfId="8" builtinId="25" customBuiltin="1"/>
     <cellStyle name="计算" xfId="9" builtinId="22" customBuiltin="1"/>
@@ -827,6 +1343,47 @@
     <cellStyle name="已访问的超链接" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1229,17 +1786,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="51.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
@@ -1251,37 +1809,37 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:10" ht="23" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1289,20 +1847,23 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -1313,20 +1874,20 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -1336,17 +1897,19 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="4">
-        <v>5000</v>
-      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
@@ -1356,18 +1919,18 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
-        <v>44</v>
+      <c r="D5" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
@@ -1377,18 +1940,21 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>44</v>
+      <c r="D6" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>43</v>
+        <v>53</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
@@ -1398,17 +1964,19 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="4">
-        <v>5000</v>
-      </c>
+      <c r="D7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
@@ -1418,11 +1986,18 @@
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
@@ -1432,8 +2007,18 @@
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
@@ -1443,6 +2028,16 @@
       <c r="B10">
         <v>8</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="4"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
@@ -1452,6 +2047,15 @@
       <c r="B11">
         <v>9</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
@@ -1461,15 +2065,34 @@
       <c r="B12">
         <v>10</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12">
+        <v>655000</v>
+      </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>0</v>
       </c>
-      <c r="B13">
-        <v>11</v>
-      </c>
+      <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="7"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
@@ -1479,6 +2102,16 @@
       <c r="B14">
         <v>12</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="2"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
@@ -1488,170 +2121,1138 @@
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>0</v>
       </c>
-      <c r="B16">
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="5"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
         <v>14</v>
       </c>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23">
+        <v>720</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24">
+        <v>1080</v>
+      </c>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="4">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="4">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G26">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
         <v>2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44">
+        <v>7</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>4</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>4</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G54" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A59">
+        <v>4</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A63">
+        <v>5</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <v>5</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A65">
+        <v>5</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A66">
+        <v>5</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A67">
+        <v>5</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A68">
+        <v>5</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A69">
+        <v>6</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A70">
+        <v>6</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G70" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A71">
+        <v>6</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A72">
+        <v>6</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A73">
+        <v>6</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A74">
+        <v>6</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A75">
+        <v>6</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A76">
+        <v>6</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A77">
+        <v>7</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A78">
+        <v>7</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G78" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A79">
+        <v>7</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A80">
+        <v>7</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A81">
+        <v>7</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A82">
+        <v>7</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H82" s="2"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A83">
+        <v>7</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A84">
+        <v>7</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1676,81 +3277,81 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2"/>
     </row>

</xml_diff>